<commit_message>
added method to translate plot table. it changed a lot in the form file
</commit_message>
<xml_diff>
--- a/src/configurations/configuration.xlsx
+++ b/src/configurations/configuration.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>parameter</t>
   </si>
@@ -40,12 +40,12 @@
     <t>database_user</t>
   </si>
   <si>
-    <t>localhost</t>
-  </si>
-  <si>
     <t>type_process</t>
   </si>
   <si>
+    <t>full</t>
+  </si>
+  <si>
     <t>database_pwd</t>
   </si>
   <si>
@@ -55,6 +55,9 @@
     <t>database_schema</t>
   </si>
   <si>
+    <t>aeps_2_0</t>
+  </si>
+  <si>
     <t>table</t>
   </si>
   <si>
@@ -95,6 +98,24 @@
   </si>
   <si>
     <t>person-document</t>
+  </si>
+  <si>
+    <t>far_farms</t>
+  </si>
+  <si>
+    <t>farmer-document</t>
+  </si>
+  <si>
+    <t>far_plots</t>
+  </si>
+  <si>
+    <t>farm-ext_id</t>
+  </si>
+  <si>
+    <t>far_production_events</t>
+  </si>
+  <si>
+    <t>plot-ext_id</t>
   </si>
 </sst>
 </file>
@@ -443,7 +464,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,25 +494,25 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
-        <v>3306</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -502,73 +523,113 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -578,10 +639,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,18 +654,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -615,7 +676,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -626,7 +687,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -637,7 +698,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -648,7 +709,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -659,12 +720,45 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working in new records
</commit_message>
<xml_diff>
--- a/src/configurations/configuration.xlsx
+++ b/src/configurations/configuration.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>parameter</t>
   </si>
@@ -40,6 +40,9 @@
     <t>database_user</t>
   </si>
   <si>
+    <t>localhost</t>
+  </si>
+  <si>
     <t>type_process</t>
   </si>
   <si>
@@ -116,6 +119,30 @@
   </si>
   <si>
     <t>plot-ext_id</t>
+  </si>
+  <si>
+    <t>far_responses_bool</t>
+  </si>
+  <si>
+    <t>far_responses_date</t>
+  </si>
+  <si>
+    <t>far_responses_numeric</t>
+  </si>
+  <si>
+    <t>far_responses_options</t>
+  </si>
+  <si>
+    <t>far_responses_text</t>
+  </si>
+  <si>
+    <t>event-plot</t>
+  </si>
+  <si>
+    <t>technical-person</t>
+  </si>
+  <si>
+    <t>technical-document</t>
   </si>
 </sst>
 </file>
@@ -464,7 +491,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,33 +514,39 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5">
+        <v>3306</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -523,113 +556,174 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H6" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
       <c r="J9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>28</v>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -639,33 +733,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A11" sqref="A11:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -676,7 +770,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -687,7 +781,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -698,7 +792,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -709,7 +803,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -720,7 +814,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -731,7 +825,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -742,7 +836,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -753,13 +847,68 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing bugs of the etl
</commit_message>
<xml_diff>
--- a/src/configurations/configuration.xlsx
+++ b/src/configurations/configuration.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
   <si>
     <t>parameter</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>technical-document</t>
+  </si>
+  <si>
+    <t>event-ext_id</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +562,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -681,24 +684,39 @@
         <v>30</v>
       </c>
       <c r="K9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="L9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="N9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="O9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
+      </c>
+      <c r="K10" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fixed some issues about importation process
</commit_message>
<xml_diff>
--- a/src/configurations/configuration.xlsx
+++ b/src/configurations/configuration.xlsx
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="global" sheetId="1" r:id="rId1"/>
-    <sheet name="dependencies" sheetId="2" r:id="rId2"/>
-    <sheet name="additional" sheetId="3" r:id="rId3"/>
+    <sheet name="dependencies" sheetId="4" r:id="rId2"/>
+    <sheet name="dependencies-1" sheetId="2" r:id="rId3"/>
+    <sheet name="additional" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="54">
   <si>
     <t>parameter</t>
   </si>
@@ -100,15 +101,9 @@
     <t>association-ext_id</t>
   </si>
   <si>
-    <t>person-document</t>
-  </si>
-  <si>
     <t>far_farms</t>
   </si>
   <si>
-    <t>farmer-document</t>
-  </si>
-  <si>
     <t>far_plots</t>
   </si>
   <si>
@@ -139,13 +134,61 @@
     <t>event-plot</t>
   </si>
   <si>
-    <t>technical-person</t>
-  </si>
-  <si>
-    <t>technical-document</t>
-  </si>
-  <si>
     <t>event-ext_id</t>
+  </si>
+  <si>
+    <t>farmer-ext_id</t>
+  </si>
+  <si>
+    <t>person-ext_id</t>
+  </si>
+  <si>
+    <t>parent_table</t>
+  </si>
+  <si>
+    <t>child_table</t>
+  </si>
+  <si>
+    <t>parent_field</t>
+  </si>
+  <si>
+    <t>child_field</t>
+  </si>
+  <si>
+    <t>ext_id</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>municipality</t>
+  </si>
+  <si>
+    <t>association</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>farmer</t>
+  </si>
+  <si>
+    <t>farm</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>technical</t>
+  </si>
+  <si>
+    <t>plot</t>
+  </si>
+  <si>
+    <t>event</t>
   </si>
 </sst>
 </file>
@@ -494,7 +537,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,194 +597,318 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="s">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="H6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="J7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" t="s">
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
         <v>30</v>
       </c>
-      <c r="K9" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" t="s">
-        <v>39</v>
-      </c>
-      <c r="M9" t="s">
-        <v>39</v>
-      </c>
-      <c r="N9" t="s">
-        <v>39</v>
-      </c>
-      <c r="O9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="K10" t="s">
-        <v>36</v>
-      </c>
-      <c r="L10" t="s">
-        <v>36</v>
-      </c>
-      <c r="M10" t="s">
-        <v>36</v>
-      </c>
-      <c r="N10" t="s">
-        <v>36</v>
-      </c>
-      <c r="O10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>35</v>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -751,10 +918,212 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A15"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,7 +1212,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -854,7 +1223,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -865,7 +1234,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -876,7 +1245,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -887,7 +1256,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -898,7 +1267,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -909,7 +1278,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -920,7 +1289,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>0</v>

</xml_diff>